<commit_message>
update PR file for week6
</commit_message>
<xml_diff>
--- a/PR/Week06_PR_F14a_T01.xlsx
+++ b/PR/Week06_PR_F14a_T01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-25600" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SLOC" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="143">
   <si>
     <t>Team Number:</t>
   </si>
@@ -271,33 +271,18 @@
     <t>PHP</t>
   </si>
   <si>
+    <t>Joomla</t>
+  </si>
+  <si>
     <t>x</t>
   </si>
   <si>
-    <t>Joomla</t>
-  </si>
-  <si>
-    <t>CMS</t>
-  </si>
-  <si>
-    <t>PHP</t>
+    <t>Wordpress</t>
   </si>
   <si>
     <t>x</t>
   </si>
   <si>
-    <t>Wordpress</t>
-  </si>
-  <si>
-    <t>CMS</t>
-  </si>
-  <si>
-    <t>PHP</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>Jquery</t>
   </si>
   <si>
@@ -307,19 +292,10 @@
     <t>Javascript</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>Bootstrap</t>
   </si>
   <si>
     <t>UI library (template system)</t>
-  </si>
-  <si>
-    <t>Javascript</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <t>Components that were filtered in the previous week</t>
@@ -476,6 +452,12 @@
   </si>
   <si>
     <t>Develop prototypes to explain new strategy to the clients and obtain feedback</t>
+  </si>
+  <si>
+    <t>Finalize documents for FCP</t>
+  </si>
+  <si>
+    <t>Develop system architecture</t>
   </si>
 </sst>
 </file>
@@ -485,7 +467,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -568,6 +550,18 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1592,8 +1586,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1779,94 +1783,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1942,8 +1858,106 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2648,8 +2662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2785,13 +2799,13 @@
       <c r="B7" s="78">
         <v>1</v>
       </c>
-      <c r="C7" s="83" t="s">
+      <c r="C7" s="126" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="85"/>
+      <c r="D7" s="127"/>
+      <c r="E7" s="127"/>
+      <c r="F7" s="127"/>
+      <c r="G7" s="128"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -2808,13 +2822,13 @@
         <f t="shared" ref="B8:B14" si="0">B7+1</f>
         <v>2</v>
       </c>
-      <c r="C8" s="83" t="s">
-        <v>121</v>
-      </c>
-      <c r="D8" s="84"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="85"/>
+      <c r="C8" s="126" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="127"/>
+      <c r="E8" s="127"/>
+      <c r="F8" s="127"/>
+      <c r="G8" s="128"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -2831,13 +2845,13 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C9" s="83" t="s">
-        <v>122</v>
-      </c>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="85"/>
+      <c r="C9" s="126" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="127"/>
+      <c r="E9" s="127"/>
+      <c r="F9" s="127"/>
+      <c r="G9" s="128"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -2854,13 +2868,13 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C10" s="83" t="s">
+      <c r="C10" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="85"/>
+      <c r="D10" s="127"/>
+      <c r="E10" s="127"/>
+      <c r="F10" s="127"/>
+      <c r="G10" s="128"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -2877,13 +2891,13 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C11" s="83" t="s">
-        <v>123</v>
-      </c>
-      <c r="D11" s="84"/>
-      <c r="E11" s="84"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="85"/>
+      <c r="C11" s="126" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="127"/>
+      <c r="E11" s="127"/>
+      <c r="F11" s="127"/>
+      <c r="G11" s="128"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -2900,11 +2914,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C12" s="83"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="84"/>
-      <c r="G12" s="85"/>
+      <c r="C12" s="126" t="s">
+        <v>141</v>
+      </c>
+      <c r="D12" s="127"/>
+      <c r="E12" s="127"/>
+      <c r="F12" s="127"/>
+      <c r="G12" s="128"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -2921,11 +2937,13 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C13" s="83"/>
-      <c r="D13" s="84"/>
-      <c r="E13" s="84"/>
-      <c r="F13" s="84"/>
-      <c r="G13" s="85"/>
+      <c r="C13" s="126" t="s">
+        <v>142</v>
+      </c>
+      <c r="D13" s="127"/>
+      <c r="E13" s="127"/>
+      <c r="F13" s="127"/>
+      <c r="G13" s="128"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -2942,11 +2960,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C14" s="89"/>
-      <c r="D14" s="87"/>
-      <c r="E14" s="87"/>
-      <c r="F14" s="87"/>
-      <c r="G14" s="88"/>
+      <c r="C14" s="132"/>
+      <c r="D14" s="130"/>
+      <c r="E14" s="130"/>
+      <c r="F14" s="130"/>
+      <c r="G14" s="131"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -3002,13 +3020,13 @@
       <c r="B17" s="78">
         <v>1</v>
       </c>
-      <c r="C17" s="83" t="s">
-        <v>124</v>
-      </c>
-      <c r="D17" s="84"/>
-      <c r="E17" s="84"/>
-      <c r="F17" s="84"/>
-      <c r="G17" s="85"/>
+      <c r="C17" s="126" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="127"/>
+      <c r="E17" s="127"/>
+      <c r="F17" s="127"/>
+      <c r="G17" s="128"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -3025,13 +3043,13 @@
         <f>B17+1</f>
         <v>2</v>
       </c>
-      <c r="C18" s="83" t="s">
-        <v>125</v>
-      </c>
-      <c r="D18" s="84"/>
-      <c r="E18" s="84"/>
-      <c r="F18" s="84"/>
-      <c r="G18" s="85"/>
+      <c r="C18" s="126" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18" s="127"/>
+      <c r="E18" s="127"/>
+      <c r="F18" s="127"/>
+      <c r="G18" s="128"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -3048,11 +3066,11 @@
         <f>B18+1</f>
         <v>3</v>
       </c>
-      <c r="C19" s="83"/>
-      <c r="D19" s="84"/>
-      <c r="E19" s="84"/>
-      <c r="F19" s="84"/>
-      <c r="G19" s="85"/>
+      <c r="C19" s="126"/>
+      <c r="D19" s="127"/>
+      <c r="E19" s="127"/>
+      <c r="F19" s="127"/>
+      <c r="G19" s="128"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -3069,11 +3087,11 @@
         <f>B19+1</f>
         <v>4</v>
       </c>
-      <c r="C20" s="83"/>
-      <c r="D20" s="84"/>
-      <c r="E20" s="84"/>
-      <c r="F20" s="84"/>
-      <c r="G20" s="85"/>
+      <c r="C20" s="126"/>
+      <c r="D20" s="127"/>
+      <c r="E20" s="127"/>
+      <c r="F20" s="127"/>
+      <c r="G20" s="128"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -3090,13 +3108,13 @@
         <f>B20+1</f>
         <v>5</v>
       </c>
-      <c r="C21" s="86" t="s">
+      <c r="C21" s="129" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="87"/>
-      <c r="E21" s="87"/>
-      <c r="F21" s="87"/>
-      <c r="G21" s="88"/>
+      <c r="D21" s="130"/>
+      <c r="E21" s="130"/>
+      <c r="F21" s="130"/>
+      <c r="G21" s="131"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -3152,13 +3170,13 @@
       <c r="B24" s="78">
         <v>1</v>
       </c>
-      <c r="C24" s="83" t="s">
-        <v>126</v>
-      </c>
-      <c r="D24" s="84"/>
-      <c r="E24" s="84"/>
-      <c r="F24" s="84"/>
-      <c r="G24" s="85"/>
+      <c r="C24" s="126" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" s="127"/>
+      <c r="E24" s="127"/>
+      <c r="F24" s="127"/>
+      <c r="G24" s="128"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -3175,13 +3193,13 @@
         <f t="shared" ref="B25:B31" si="1">B24+1</f>
         <v>2</v>
       </c>
-      <c r="C25" s="83" t="s">
-        <v>127</v>
-      </c>
-      <c r="D25" s="84"/>
-      <c r="E25" s="84"/>
-      <c r="F25" s="84"/>
-      <c r="G25" s="85"/>
+      <c r="C25" s="126" t="s">
+        <v>119</v>
+      </c>
+      <c r="D25" s="127"/>
+      <c r="E25" s="127"/>
+      <c r="F25" s="127"/>
+      <c r="G25" s="128"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -3198,13 +3216,13 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="C26" s="83" t="s">
-        <v>128</v>
-      </c>
-      <c r="D26" s="84"/>
-      <c r="E26" s="84"/>
-      <c r="F26" s="84"/>
-      <c r="G26" s="85"/>
+      <c r="C26" s="126" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26" s="127"/>
+      <c r="E26" s="127"/>
+      <c r="F26" s="127"/>
+      <c r="G26" s="128"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -3221,13 +3239,13 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="C27" s="83" t="s">
-        <v>129</v>
-      </c>
-      <c r="D27" s="84"/>
-      <c r="E27" s="84"/>
-      <c r="F27" s="84"/>
-      <c r="G27" s="85"/>
+      <c r="C27" s="126" t="s">
+        <v>121</v>
+      </c>
+      <c r="D27" s="127"/>
+      <c r="E27" s="127"/>
+      <c r="F27" s="127"/>
+      <c r="G27" s="128"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -3244,13 +3262,13 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="C28" s="83" t="s">
-        <v>130</v>
-      </c>
-      <c r="D28" s="84"/>
-      <c r="E28" s="84"/>
-      <c r="F28" s="84"/>
-      <c r="G28" s="85"/>
+      <c r="C28" s="126" t="s">
+        <v>122</v>
+      </c>
+      <c r="D28" s="127"/>
+      <c r="E28" s="127"/>
+      <c r="F28" s="127"/>
+      <c r="G28" s="128"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -3267,13 +3285,13 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="C29" s="83" t="s">
-        <v>131</v>
-      </c>
-      <c r="D29" s="84"/>
-      <c r="E29" s="84"/>
-      <c r="F29" s="84"/>
-      <c r="G29" s="85"/>
+      <c r="C29" s="126" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="127"/>
+      <c r="E29" s="127"/>
+      <c r="F29" s="127"/>
+      <c r="G29" s="128"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -3290,11 +3308,11 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="C30" s="83"/>
-      <c r="D30" s="84"/>
-      <c r="E30" s="84"/>
-      <c r="F30" s="84"/>
-      <c r="G30" s="85"/>
+      <c r="C30" s="126"/>
+      <c r="D30" s="127"/>
+      <c r="E30" s="127"/>
+      <c r="F30" s="127"/>
+      <c r="G30" s="128"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -3311,11 +3329,11 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="C31" s="86"/>
-      <c r="D31" s="87"/>
-      <c r="E31" s="87"/>
-      <c r="F31" s="87"/>
-      <c r="G31" s="88"/>
+      <c r="C31" s="129"/>
+      <c r="D31" s="130"/>
+      <c r="E31" s="130"/>
+      <c r="F31" s="130"/>
+      <c r="G31" s="131"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -4057,8 +4075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -4094,16 +4112,16 @@
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="133" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="92"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="135"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -4117,14 +4135,14 @@
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="93"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="95"/>
+      <c r="B3" s="136"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="137"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="138"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -4138,14 +4156,14 @@
     </row>
     <row r="4" spans="1:19" ht="15" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="96"/>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="97"/>
-      <c r="I4" s="98"/>
+      <c r="B4" s="139"/>
+      <c r="C4" s="140"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="140"/>
+      <c r="F4" s="140"/>
+      <c r="G4" s="140"/>
+      <c r="H4" s="140"/>
+      <c r="I4" s="141"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -4159,26 +4177,26 @@
     </row>
     <row r="5" spans="1:19" ht="15" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="99" t="s">
+      <c r="B5" s="142" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="100"/>
-      <c r="D5" s="101" t="s">
+      <c r="C5" s="143"/>
+      <c r="D5" s="144" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="102" t="s">
+      <c r="E5" s="145" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="104" t="s">
+      <c r="F5" s="147" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="104" t="s">
+      <c r="G5" s="147" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="104" t="s">
+      <c r="H5" s="147" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="103" t="s">
+      <c r="I5" s="146" t="s">
         <v>43</v>
       </c>
       <c r="J5" s="1"/>
@@ -4200,12 +4218,12 @@
       <c r="C6" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="100"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="105"/>
-      <c r="G6" s="105"/>
-      <c r="H6" s="105"/>
-      <c r="I6" s="98"/>
+      <c r="D6" s="143"/>
+      <c r="E6" s="139"/>
+      <c r="F6" s="148"/>
+      <c r="G6" s="148"/>
+      <c r="H6" s="148"/>
+      <c r="I6" s="141"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -4225,10 +4243,10 @@
       <c r="C7" s="19">
         <v>1</v>
       </c>
-      <c r="D7" s="127" t="s">
-        <v>132</v>
-      </c>
-      <c r="E7" s="128" t="s">
+      <c r="D7" s="83" t="s">
+        <v>124</v>
+      </c>
+      <c r="E7" s="84" t="s">
         <v>46</v>
       </c>
       <c r="F7" s="20">
@@ -4237,7 +4255,7 @@
       <c r="G7" s="20">
         <v>9</v>
       </c>
-      <c r="H7" s="132">
+      <c r="H7" s="88">
         <f t="shared" ref="H7:H14" si="0">F7*G7</f>
         <v>72</v>
       </c>
@@ -4263,10 +4281,10 @@
       <c r="C8" s="23">
         <v>4</v>
       </c>
-      <c r="D8" s="134" t="s">
+      <c r="D8" s="90" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="129" t="s">
+      <c r="E8" s="85" t="s">
         <v>52</v>
       </c>
       <c r="F8" s="20">
@@ -4275,7 +4293,7 @@
       <c r="G8" s="20">
         <v>10</v>
       </c>
-      <c r="H8" s="132">
+      <c r="H8" s="88">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
@@ -4298,10 +4316,10 @@
       <c r="C9" s="23">
         <v>2</v>
       </c>
-      <c r="D9" s="127" t="s">
+      <c r="D9" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="129" t="s">
+      <c r="E9" s="85" t="s">
         <v>48</v>
       </c>
       <c r="F9" s="20">
@@ -4310,7 +4328,7 @@
       <c r="G9" s="20">
         <v>10</v>
       </c>
-      <c r="H9" s="132">
+      <c r="H9" s="88">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
@@ -4332,10 +4350,10 @@
       <c r="C10" s="23">
         <v>7</v>
       </c>
-      <c r="D10" s="127" t="s">
+      <c r="D10" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="129" t="s">
+      <c r="E10" s="85" t="s">
         <v>57</v>
       </c>
       <c r="F10" s="20">
@@ -4344,7 +4362,7 @@
       <c r="G10" s="20">
         <v>8</v>
       </c>
-      <c r="H10" s="132">
+      <c r="H10" s="88">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
@@ -4367,10 +4385,10 @@
       <c r="C11" s="23">
         <v>6</v>
       </c>
-      <c r="D11" s="127" t="s">
+      <c r="D11" s="83" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="127" t="s">
+      <c r="E11" s="83" t="s">
         <v>55</v>
       </c>
       <c r="F11" s="25">
@@ -4379,7 +4397,7 @@
       <c r="G11" s="25">
         <v>8</v>
       </c>
-      <c r="H11" s="132">
+      <c r="H11" s="88">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
@@ -4401,10 +4419,10 @@
       <c r="C12" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="130" t="s">
-        <v>133</v>
-      </c>
-      <c r="E12" s="129" t="s">
+      <c r="D12" s="86" t="s">
+        <v>125</v>
+      </c>
+      <c r="E12" s="85" t="s">
         <v>50</v>
       </c>
       <c r="F12" s="20">
@@ -4413,7 +4431,7 @@
       <c r="G12" s="20">
         <v>7</v>
       </c>
-      <c r="H12" s="132">
+      <c r="H12" s="88">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
@@ -4440,10 +4458,10 @@
       <c r="C13" s="23">
         <v>3</v>
       </c>
-      <c r="D13" s="127" t="s">
+      <c r="D13" s="83" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="129" t="s">
+      <c r="E13" s="85" t="s">
         <v>50</v>
       </c>
       <c r="F13" s="20">
@@ -4452,7 +4470,7 @@
       <c r="G13" s="20">
         <v>3</v>
       </c>
-      <c r="H13" s="132">
+      <c r="H13" s="88">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
@@ -4479,11 +4497,11 @@
       <c r="C14" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="135" t="s">
-        <v>134</v>
-      </c>
-      <c r="E14" s="135" t="s">
-        <v>135</v>
+      <c r="D14" s="91" t="s">
+        <v>126</v>
+      </c>
+      <c r="E14" s="91" t="s">
+        <v>127</v>
       </c>
       <c r="F14" s="25">
         <v>4</v>
@@ -4491,7 +4509,7 @@
       <c r="G14" s="25">
         <v>2</v>
       </c>
-      <c r="H14" s="131">
+      <c r="H14" s="87">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -4523,7 +4541,7 @@
       <c r="F15" s="26"/>
       <c r="G15" s="26"/>
       <c r="H15" s="26"/>
-      <c r="I15" s="133"/>
+      <c r="I15" s="89"/>
       <c r="J15" s="82"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -4670,7 +4688,7 @@
   <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -4708,15 +4726,15 @@
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="122" t="s">
+      <c r="B2" s="165" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
+      <c r="H2" s="143"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -4756,15 +4774,15 @@
       <c r="C4" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="118" t="s">
+      <c r="D4" s="161" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="119"/>
-      <c r="F4" s="120" t="s">
+      <c r="E4" s="162"/>
+      <c r="F4" s="163" t="s">
         <v>65</v>
       </c>
-      <c r="G4" s="119"/>
-      <c r="H4" s="121"/>
+      <c r="G4" s="162"/>
+      <c r="H4" s="164"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -4862,20 +4880,20 @@
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="40" t="s">
+      <c r="B8" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="46" t="s">
         <v>80</v>
       </c>
       <c r="E8" s="43"/>
       <c r="F8" s="37"/>
       <c r="G8" s="37"/>
       <c r="H8" s="44" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -4891,19 +4909,19 @@
     <row r="9" spans="1:18" ht="15" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="46" t="s">
-        <v>84</v>
+      <c r="C9" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>80</v>
       </c>
       <c r="E9" s="47"/>
       <c r="F9" s="37"/>
       <c r="G9" s="37"/>
       <c r="H9" s="44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -4919,20 +4937,20 @@
     <row r="10" spans="1:18" ht="15" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="D10" s="48" t="s">
         <v>87</v>
-      </c>
-      <c r="D10" s="40" t="s">
-        <v>88</v>
       </c>
       <c r="E10" s="47"/>
       <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="44" t="s">
-        <v>89</v>
-      </c>
+      <c r="G10" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" s="44"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -4946,19 +4964,19 @@
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="45" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" s="40" t="s">
-        <v>91</v>
+      <c r="B11" s="49" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>89</v>
       </c>
       <c r="D11" s="48" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E11" s="47"/>
       <c r="F11" s="36"/>
-      <c r="G11" s="36" t="s">
-        <v>93</v>
+      <c r="G11" s="51" t="s">
+        <v>74</v>
       </c>
       <c r="H11" s="38"/>
       <c r="I11" s="1"/>
@@ -4974,20 +4992,12 @@
     </row>
     <row r="12" spans="1:18" ht="15.75" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="49" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="D12" s="48" t="s">
-        <v>96</v>
-      </c>
+      <c r="B12" s="49"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="48"/>
       <c r="E12" s="50"/>
       <c r="F12" s="51"/>
-      <c r="G12" s="51" t="s">
-        <v>97</v>
-      </c>
+      <c r="G12" s="51"/>
       <c r="H12" s="52"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -5042,15 +5052,15 @@
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="122" t="s">
-        <v>98</v>
-      </c>
-      <c r="C15" s="100"/>
-      <c r="D15" s="100"/>
-      <c r="E15" s="100"/>
-      <c r="F15" s="100"/>
-      <c r="G15" s="100"/>
-      <c r="H15" s="100"/>
+      <c r="B15" s="165" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="143"/>
+      <c r="D15" s="143"/>
+      <c r="E15" s="143"/>
+      <c r="F15" s="143"/>
+      <c r="G15" s="143"/>
+      <c r="H15" s="143"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -5085,18 +5095,18 @@
     <row r="17" spans="1:18" ht="51" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="57" t="s">
-        <v>99</v>
-      </c>
-      <c r="C17" s="114" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" s="115"/>
-      <c r="E17" s="116" t="s">
-        <v>101</v>
-      </c>
-      <c r="F17" s="117"/>
-      <c r="G17" s="117"/>
-      <c r="H17" s="115"/>
+        <v>91</v>
+      </c>
+      <c r="C17" s="157" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="158"/>
+      <c r="E17" s="159" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" s="160"/>
+      <c r="G17" s="160"/>
+      <c r="H17" s="158"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -5113,16 +5123,16 @@
       <c r="B18" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="108" t="s">
-        <v>136</v>
-      </c>
-      <c r="D18" s="85"/>
-      <c r="E18" s="108" t="s">
-        <v>137</v>
-      </c>
-      <c r="F18" s="84"/>
-      <c r="G18" s="84"/>
-      <c r="H18" s="85"/>
+      <c r="C18" s="151" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" s="128"/>
+      <c r="E18" s="151" t="s">
+        <v>129</v>
+      </c>
+      <c r="F18" s="127"/>
+      <c r="G18" s="127"/>
+      <c r="H18" s="128"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -5137,12 +5147,12 @@
     <row r="19" spans="1:18" ht="15" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="59"/>
-      <c r="C19" s="109"/>
-      <c r="D19" s="110"/>
-      <c r="E19" s="106"/>
-      <c r="F19" s="84"/>
-      <c r="G19" s="84"/>
-      <c r="H19" s="85"/>
+      <c r="C19" s="152"/>
+      <c r="D19" s="153"/>
+      <c r="E19" s="149"/>
+      <c r="F19" s="127"/>
+      <c r="G19" s="127"/>
+      <c r="H19" s="128"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -5157,12 +5167,12 @@
     <row r="20" spans="1:18" ht="15" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="59"/>
-      <c r="C20" s="111"/>
-      <c r="D20" s="85"/>
-      <c r="E20" s="106"/>
-      <c r="F20" s="84"/>
-      <c r="G20" s="84"/>
-      <c r="H20" s="85"/>
+      <c r="C20" s="154"/>
+      <c r="D20" s="128"/>
+      <c r="E20" s="149"/>
+      <c r="F20" s="127"/>
+      <c r="G20" s="127"/>
+      <c r="H20" s="128"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -5177,12 +5187,12 @@
     <row r="21" spans="1:18" ht="15" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="60"/>
-      <c r="C21" s="112"/>
-      <c r="D21" s="85"/>
-      <c r="E21" s="106"/>
-      <c r="F21" s="84"/>
-      <c r="G21" s="84"/>
-      <c r="H21" s="85"/>
+      <c r="C21" s="155"/>
+      <c r="D21" s="128"/>
+      <c r="E21" s="149"/>
+      <c r="F21" s="127"/>
+      <c r="G21" s="127"/>
+      <c r="H21" s="128"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -5197,12 +5207,12 @@
     <row r="22" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
       <c r="A22" s="1"/>
       <c r="B22" s="61"/>
-      <c r="C22" s="113"/>
-      <c r="D22" s="88"/>
-      <c r="E22" s="107"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="87"/>
-      <c r="H22" s="88"/>
+      <c r="C22" s="156"/>
+      <c r="D22" s="131"/>
+      <c r="E22" s="150"/>
+      <c r="F22" s="130"/>
+      <c r="G22" s="130"/>
+      <c r="H22" s="131"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -5234,6 +5244,7 @@
     <mergeCell ref="C18:D18"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5277,10 +5288,10 @@
     </row>
     <row r="2" spans="1:14" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="125" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" s="100"/>
+      <c r="B2" s="168" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="143"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -5295,10 +5306,10 @@
     </row>
     <row r="3" spans="1:14" ht="12" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="126" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" s="100"/>
+      <c r="B3" s="169" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="143"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -5329,11 +5340,11 @@
     </row>
     <row r="5" spans="1:14" ht="12" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="124" t="s">
-        <v>104</v>
-      </c>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
+      <c r="B5" s="167" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="143"/>
+      <c r="D5" s="143"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -5347,11 +5358,11 @@
     </row>
     <row r="6" spans="1:14" ht="12" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="124" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" s="100"/>
-      <c r="D6" s="100"/>
+      <c r="B6" s="167" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="143"/>
+      <c r="D6" s="143"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -5365,11 +5376,11 @@
     </row>
     <row r="7" spans="1:14" ht="12" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="123" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" s="100"/>
-      <c r="D7" s="100"/>
+      <c r="B7" s="166" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="143"/>
+      <c r="D7" s="143"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -5416,7 +5427,7 @@
     <row r="10" spans="1:14" ht="12.75" customHeight="1" thickBot="1">
       <c r="A10" s="1"/>
       <c r="B10" s="12" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -5433,12 +5444,12 @@
     </row>
     <row r="11" spans="1:14" ht="12.75" customHeight="1" thickBot="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="161"/>
-      <c r="C11" s="148" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" s="151" t="s">
-        <v>109</v>
+      <c r="B11" s="117"/>
+      <c r="C11" s="104" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="107" t="s">
+        <v>101</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -5453,14 +5464,14 @@
     </row>
     <row r="12" spans="1:14" ht="12" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="162">
+      <c r="B12" s="118">
         <v>1</v>
       </c>
-      <c r="C12" s="156" t="s">
-        <v>138</v>
-      </c>
-      <c r="D12" s="152" t="s">
-        <v>140</v>
+      <c r="C12" s="112" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" s="108" t="s">
+        <v>132</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -5479,11 +5490,11 @@
         <f>B12+1</f>
         <v>2</v>
       </c>
-      <c r="C13" s="157" t="s">
-        <v>139</v>
-      </c>
-      <c r="D13" s="153" t="s">
-        <v>141</v>
+      <c r="C13" s="113" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" s="109" t="s">
+        <v>133</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -5502,7 +5513,7 @@
         <f>B13+1</f>
         <v>3</v>
       </c>
-      <c r="C14" s="158"/>
+      <c r="C14" s="114"/>
       <c r="D14" s="70"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -5521,8 +5532,8 @@
         <f>B14+1</f>
         <v>4</v>
       </c>
-      <c r="C15" s="159"/>
-      <c r="D15" s="154"/>
+      <c r="C15" s="115"/>
+      <c r="D15" s="110"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -5540,8 +5551,8 @@
         <f>B15+1</f>
         <v>5</v>
       </c>
-      <c r="C16" s="160"/>
-      <c r="D16" s="155"/>
+      <c r="C16" s="116"/>
+      <c r="D16" s="111"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -5588,7 +5599,7 @@
     <row r="19" spans="1:14" ht="12.75" customHeight="1" thickBot="1">
       <c r="A19" s="1"/>
       <c r="B19" s="12" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -5605,12 +5616,12 @@
     </row>
     <row r="20" spans="1:14" ht="12.75" customHeight="1" thickBot="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="167"/>
-      <c r="C20" s="137" t="s">
-        <v>111</v>
-      </c>
-      <c r="D20" s="148" t="s">
-        <v>112</v>
+      <c r="B20" s="123"/>
+      <c r="C20" s="93" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="104" t="s">
+        <v>104</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -5625,14 +5636,14 @@
     </row>
     <row r="21" spans="1:14" ht="12" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="168">
+      <c r="B21" s="124">
         <v>1</v>
       </c>
-      <c r="C21" s="163" t="s">
-        <v>142</v>
-      </c>
-      <c r="D21" s="146" t="s">
-        <v>144</v>
+      <c r="C21" s="119" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" s="102" t="s">
+        <v>136</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -5651,11 +5662,11 @@
         <f>B21+1</f>
         <v>2</v>
       </c>
-      <c r="C22" s="164" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" s="142" t="s">
-        <v>145</v>
+      <c r="C22" s="120" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="98" t="s">
+        <v>137</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -5674,11 +5685,11 @@
         <f>B22+1</f>
         <v>3</v>
       </c>
-      <c r="C23" s="165" t="s">
-        <v>143</v>
-      </c>
-      <c r="D23" s="142" t="s">
-        <v>146</v>
+      <c r="C23" s="121" t="s">
+        <v>135</v>
+      </c>
+      <c r="D23" s="98" t="s">
+        <v>138</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -5697,8 +5708,8 @@
         <f>B23+1</f>
         <v>4</v>
       </c>
-      <c r="C24" s="166"/>
-      <c r="D24" s="149"/>
+      <c r="C24" s="122"/>
+      <c r="D24" s="105"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -5716,8 +5727,8 @@
         <f>B24+1</f>
         <v>5</v>
       </c>
-      <c r="C25" s="169"/>
-      <c r="D25" s="150"/>
+      <c r="C25" s="125"/>
+      <c r="D25" s="106"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -5764,7 +5775,7 @@
     <row r="28" spans="1:14" ht="12.75" customHeight="1" thickBot="1">
       <c r="A28" s="1"/>
       <c r="B28" s="12" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -5782,11 +5793,11 @@
     <row r="29" spans="1:14" ht="12.75" customHeight="1" thickBot="1">
       <c r="A29" s="1"/>
       <c r="B29" s="71"/>
-      <c r="C29" s="136" t="s">
-        <v>115</v>
-      </c>
-      <c r="D29" s="147" t="s">
-        <v>116</v>
+      <c r="C29" s="92" t="s">
+        <v>107</v>
+      </c>
+      <c r="D29" s="103" t="s">
+        <v>108</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -5804,11 +5815,11 @@
       <c r="B30" s="72">
         <v>1</v>
       </c>
-      <c r="C30" s="138" t="s">
-        <v>147</v>
-      </c>
-      <c r="D30" s="146" t="s">
-        <v>148</v>
+      <c r="C30" s="94" t="s">
+        <v>139</v>
+      </c>
+      <c r="D30" s="102" t="s">
+        <v>140</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="13"/>
@@ -5827,11 +5838,11 @@
         <f>B30+1</f>
         <v>2</v>
       </c>
-      <c r="C31" s="139" t="s">
-        <v>117</v>
-      </c>
-      <c r="D31" s="143" t="s">
-        <v>118</v>
+      <c r="C31" s="95" t="s">
+        <v>109</v>
+      </c>
+      <c r="D31" s="99" t="s">
+        <v>110</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="13"/>
@@ -5850,11 +5861,11 @@
         <f>B31+1</f>
         <v>3</v>
       </c>
-      <c r="C32" s="139" t="s">
-        <v>119</v>
-      </c>
-      <c r="D32" s="144" t="s">
-        <v>120</v>
+      <c r="C32" s="95" t="s">
+        <v>111</v>
+      </c>
+      <c r="D32" s="100" t="s">
+        <v>112</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="13"/>
@@ -5873,8 +5884,8 @@
         <f>B32+1</f>
         <v>4</v>
       </c>
-      <c r="C33" s="140"/>
-      <c r="D33" s="143"/>
+      <c r="C33" s="96"/>
+      <c r="D33" s="99"/>
       <c r="E33" s="1"/>
       <c r="F33" s="13"/>
       <c r="G33" s="1"/>
@@ -5892,8 +5903,8 @@
         <f>B33+1</f>
         <v>5</v>
       </c>
-      <c r="C34" s="141"/>
-      <c r="D34" s="145"/>
+      <c r="C34" s="97"/>
+      <c r="D34" s="101"/>
       <c r="E34" s="56"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>

</xml_diff>